<commit_message>
qmm019p: update file template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/明細レイアウトの作成.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/明細レイアウトの作成.xlsx
@@ -52,6 +52,33 @@
     <definedName name="AAAA" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="abc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ADD_COPY句">#N/A</definedName>
+    <definedName name="attendItem1">'出力イメージ '!$B$18:$B$20</definedName>
+    <definedName name="attendItem1_info1">'出力イメージ '!$B$19</definedName>
+    <definedName name="attendItem1_info2">'出力イメージ '!$B$20</definedName>
+    <definedName name="attendItem2">'出力イメージ '!$C$18:$C$20</definedName>
+    <definedName name="attendItem2_info1">'出力イメージ '!$C$19</definedName>
+    <definedName name="attendItem2_info2">'出力イメージ '!$C$20</definedName>
+    <definedName name="attendItem3">'出力イメージ '!$D$18:$D$20</definedName>
+    <definedName name="attendItem3_info1">'出力イメージ '!$D$19</definedName>
+    <definedName name="attendItem3_info2">'出力イメージ '!$D$20</definedName>
+    <definedName name="attendItem4">'出力イメージ '!$E$18:$E$20</definedName>
+    <definedName name="attendItem4_info1">'出力イメージ '!$E$19</definedName>
+    <definedName name="attendItem4_info2">'出力イメージ '!$E$20</definedName>
+    <definedName name="attendItem5">'出力イメージ '!$F$18:$F$20</definedName>
+    <definedName name="attendItem5_info1">'出力イメージ '!$F$19</definedName>
+    <definedName name="attendItem5_info2">'出力イメージ '!$F$20</definedName>
+    <definedName name="attendItem6">'出力イメージ '!$G$18:$G$20</definedName>
+    <definedName name="attendItem6_info1">'出力イメージ '!$G$19</definedName>
+    <definedName name="attendItem6_info2">'出力イメージ '!$G$20</definedName>
+    <definedName name="attendItem7">'出力イメージ '!$H$18:$H$20</definedName>
+    <definedName name="attendItem7_info1">'出力イメージ '!$H$19</definedName>
+    <definedName name="attendItem7_info2">'出力イメージ '!$H$20</definedName>
+    <definedName name="attendItem8">'出力イメージ '!$I$18:$I$20</definedName>
+    <definedName name="attendItem8_info1">'出力イメージ '!$I$19</definedName>
+    <definedName name="attendItem8_info2">'出力イメージ '!$I$20</definedName>
+    <definedName name="attendItem9">'出力イメージ '!$J$18:$J$20</definedName>
+    <definedName name="attendItem9_info1">'出力イメージ '!$J$19</definedName>
+    <definedName name="attendItem9_info2">'出力イメージ '!$J$20</definedName>
     <definedName name="attendRow">'出力イメージ '!$A$18:$J$20</definedName>
     <definedName name="b" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
@@ -71,6 +98,78 @@
     <definedName name="C保守単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="deductionItem1">'出力イメージ '!$B$10:$B$16</definedName>
+    <definedName name="deductionItem1_info1">'出力イメージ '!$B$11</definedName>
+    <definedName name="deductionItem1_info2">'出力イメージ '!$B$12</definedName>
+    <definedName name="deductionItem1_info3">'出力イメージ '!$B$13</definedName>
+    <definedName name="deductionItem1_info4">'出力イメージ '!$B$14</definedName>
+    <definedName name="deductionItem1_info5">'出力イメージ '!$B$15</definedName>
+    <definedName name="deductionItem1_info6">'出力イメージ '!$B$16</definedName>
+    <definedName name="deductionItem1_name">'出力イメージ '!$B$10</definedName>
+    <definedName name="deductionItem2">'出力イメージ '!$C$10:$C$16</definedName>
+    <definedName name="deductionItem2_info1">'出力イメージ '!$C$11</definedName>
+    <definedName name="deductionItem2_info2">'出力イメージ '!$C$12</definedName>
+    <definedName name="deductionItem2_info3">'出力イメージ '!$C$13</definedName>
+    <definedName name="deductionItem2_info4">'出力イメージ '!$C$14</definedName>
+    <definedName name="deductionItem2_info5">'出力イメージ '!$C$15</definedName>
+    <definedName name="deductionItem2_info6">'出力イメージ '!$C$16</definedName>
+    <definedName name="deductionItem2_name">'出力イメージ '!$C$10</definedName>
+    <definedName name="deductionItem3">'出力イメージ '!$D$10:$D$16</definedName>
+    <definedName name="deductionItem3_info1">'出力イメージ '!$D$11</definedName>
+    <definedName name="deductionItem3_info2">'出力イメージ '!$D$12</definedName>
+    <definedName name="deductionItem3_info3">'出力イメージ '!$D$13</definedName>
+    <definedName name="deductionItem3_info4">'出力イメージ '!$D$14</definedName>
+    <definedName name="deductionItem3_info5">'出力イメージ '!$D$15</definedName>
+    <definedName name="deductionItem3_info6">'出力イメージ '!$D$16</definedName>
+    <definedName name="deductionItem3_name">'出力イメージ '!$D$10</definedName>
+    <definedName name="deductionItem4">'出力イメージ '!$E$10:$E$16</definedName>
+    <definedName name="deductionItem4_info1">'出力イメージ '!$E$11</definedName>
+    <definedName name="deductionItem4_info2">'出力イメージ '!$E$12</definedName>
+    <definedName name="deductionItem4_info3">'出力イメージ '!$E$13</definedName>
+    <definedName name="deductionItem4_info4">'出力イメージ '!$E$14</definedName>
+    <definedName name="deductionItem4_info5">'出力イメージ '!$E$15</definedName>
+    <definedName name="deductionItem4_info6">'出力イメージ '!$E$16</definedName>
+    <definedName name="deductionItem4_name">'出力イメージ '!$E$10</definedName>
+    <definedName name="deductionItem5">'出力イメージ '!$F$10:$F$16</definedName>
+    <definedName name="deductionItem5_info1">'出力イメージ '!$F$11</definedName>
+    <definedName name="deductionItem5_info2">'出力イメージ '!$F$12</definedName>
+    <definedName name="deductionItem5_info3">'出力イメージ '!$F$13</definedName>
+    <definedName name="deductionItem5_info4">'出力イメージ '!$F$14</definedName>
+    <definedName name="deductionItem5_info5">'出力イメージ '!$F$15</definedName>
+    <definedName name="deductionItem5_info6">'出力イメージ '!$F$16</definedName>
+    <definedName name="deductionItem5_name">'出力イメージ '!$F$10</definedName>
+    <definedName name="deductionItem6">'出力イメージ '!$G$10:$G$16</definedName>
+    <definedName name="deductionItem6_info1">'出力イメージ '!$G$11</definedName>
+    <definedName name="deductionItem6_info2">'出力イメージ '!$G$12</definedName>
+    <definedName name="deductionItem6_info3">'出力イメージ '!$G$13</definedName>
+    <definedName name="deductionItem6_info4">'出力イメージ '!$G$14</definedName>
+    <definedName name="deductionItem6_info5">'出力イメージ '!$G$15</definedName>
+    <definedName name="deductionItem6_info6">'出力イメージ '!$G$16</definedName>
+    <definedName name="deductionItem6_name">'出力イメージ '!$G$10</definedName>
+    <definedName name="deductionItem7">'出力イメージ '!$H$10:$H$16</definedName>
+    <definedName name="deductionItem7_info1">'出力イメージ '!$H$11</definedName>
+    <definedName name="deductionItem7_info2">'出力イメージ '!$H$12</definedName>
+    <definedName name="deductionItem7_info3">'出力イメージ '!$H$13</definedName>
+    <definedName name="deductionItem7_info4">'出力イメージ '!$H$14</definedName>
+    <definedName name="deductionItem7_info5">'出力イメージ '!$H$15</definedName>
+    <definedName name="deductionItem7_info6">'出力イメージ '!$H$16</definedName>
+    <definedName name="deductionItem7_name">'出力イメージ '!$H$10</definedName>
+    <definedName name="deductionItem8">'出力イメージ '!$I$10:$I$16</definedName>
+    <definedName name="deductionItem8_info1">'出力イメージ '!$I$11</definedName>
+    <definedName name="deductionItem8_info2">'出力イメージ '!$I$12</definedName>
+    <definedName name="deductionItem8_info3">'出力イメージ '!$I$13</definedName>
+    <definedName name="deductionItem8_info4">'出力イメージ '!$I$14</definedName>
+    <definedName name="deductionItem8_info5">'出力イメージ '!$I$15</definedName>
+    <definedName name="deductionItem8_info6">'出力イメージ '!$I$16</definedName>
+    <definedName name="deductionItem8_name">'出力イメージ '!$I$10</definedName>
+    <definedName name="deductionItem9">'出力イメージ '!$J$10:$J$16</definedName>
+    <definedName name="deductionItem9_info1">'出力イメージ '!$J$11</definedName>
+    <definedName name="deductionItem9_info2">'出力イメージ '!$J$12</definedName>
+    <definedName name="deductionItem9_info3">'出力イメージ '!$J$13</definedName>
+    <definedName name="deductionItem9_info4">'出力イメージ '!$J$14</definedName>
+    <definedName name="deductionItem9_info5">'出力イメージ '!$J$15</definedName>
+    <definedName name="deductionItem9_info6">'出力イメージ '!$J$16</definedName>
+    <definedName name="deductionItem9_name">'出力イメージ '!$J$10</definedName>
     <definedName name="deductionRow">'出力イメージ '!$A$10:$J$16</definedName>
     <definedName name="def" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="e" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
@@ -113,6 +212,78 @@
     <definedName name="OPT_YES">[7]!OPT_YES</definedName>
     <definedName name="Ｏホ" localSheetId="0">#REF!</definedName>
     <definedName name="Ｏホ">#REF!</definedName>
+    <definedName name="paymentItem1">'出力イメージ '!$B$2:$B$8</definedName>
+    <definedName name="paymentItem1_info1">'出力イメージ '!$B$3</definedName>
+    <definedName name="paymentItem1_info2">'出力イメージ '!$B$4</definedName>
+    <definedName name="paymentItem1_info3">'出力イメージ '!$B$5</definedName>
+    <definedName name="paymentItem1_info4">'出力イメージ '!$B$6</definedName>
+    <definedName name="paymentItem1_info5">'出力イメージ '!$B$7</definedName>
+    <definedName name="paymentItem1_info6">'出力イメージ '!$B$8</definedName>
+    <definedName name="paymentItem1_name">'出力イメージ '!$B$2</definedName>
+    <definedName name="paymentItem2">'出力イメージ '!$C$2:$C$8</definedName>
+    <definedName name="paymentItem2_info1">'出力イメージ '!$C$3</definedName>
+    <definedName name="paymentItem2_info2">'出力イメージ '!$C$4</definedName>
+    <definedName name="paymentItem2_info3">'出力イメージ '!$C$5</definedName>
+    <definedName name="paymentItem2_info4">'出力イメージ '!$C$6</definedName>
+    <definedName name="paymentItem2_info5">'出力イメージ '!$C$7</definedName>
+    <definedName name="paymentItem2_info6">'出力イメージ '!$C$8</definedName>
+    <definedName name="paymentItem2_name">'出力イメージ '!$C$2</definedName>
+    <definedName name="paymentItem3">'出力イメージ '!$D$2:$D$8</definedName>
+    <definedName name="paymentItem3_info1">'出力イメージ '!$D$3</definedName>
+    <definedName name="paymentItem3_info2">'出力イメージ '!$D$4</definedName>
+    <definedName name="paymentItem3_info3">'出力イメージ '!$D$5</definedName>
+    <definedName name="paymentItem3_info4">'出力イメージ '!$D$6</definedName>
+    <definedName name="paymentItem3_info5">'出力イメージ '!$D$7</definedName>
+    <definedName name="paymentItem3_info6">'出力イメージ '!$D$8</definedName>
+    <definedName name="paymentItem3_name">'出力イメージ '!$D$2</definedName>
+    <definedName name="paymentItem4">'出力イメージ '!$E$2:$E$8</definedName>
+    <definedName name="paymentItem4_info1">'出力イメージ '!$E$3</definedName>
+    <definedName name="paymentItem4_info2">'出力イメージ '!$E$4</definedName>
+    <definedName name="paymentItem4_info3">'出力イメージ '!$E$5</definedName>
+    <definedName name="paymentItem4_info4">'出力イメージ '!$E$6</definedName>
+    <definedName name="paymentItem4_info5">'出力イメージ '!$E$7</definedName>
+    <definedName name="paymentItem4_info6">'出力イメージ '!$E$8</definedName>
+    <definedName name="paymentItem4_name">'出力イメージ '!$E$2</definedName>
+    <definedName name="paymentItem5">'出力イメージ '!$F$2:$F$8</definedName>
+    <definedName name="paymentItem5_info1">'出力イメージ '!$F$3</definedName>
+    <definedName name="paymentItem5_info2">'出力イメージ '!$F$4</definedName>
+    <definedName name="paymentItem5_info3">'出力イメージ '!$F$5</definedName>
+    <definedName name="paymentItem5_info4">'出力イメージ '!$F$6</definedName>
+    <definedName name="paymentItem5_info5">'出力イメージ '!$F$7</definedName>
+    <definedName name="paymentItem5_info6">'出力イメージ '!$F$8</definedName>
+    <definedName name="paymentItem5_name">'出力イメージ '!$F$2</definedName>
+    <definedName name="paymentItem6">'出力イメージ '!$G$2:$G$8</definedName>
+    <definedName name="paymentItem6_info1">'出力イメージ '!$G$3</definedName>
+    <definedName name="paymentItem6_info2">'出力イメージ '!$G$4</definedName>
+    <definedName name="paymentItem6_info3">'出力イメージ '!$G$5</definedName>
+    <definedName name="paymentItem6_info4">'出力イメージ '!$G$6</definedName>
+    <definedName name="paymentItem6_info5">'出力イメージ '!$G$7</definedName>
+    <definedName name="paymentItem6_info6">'出力イメージ '!$G$8</definedName>
+    <definedName name="paymentItem6_name">'出力イメージ '!$G$2</definedName>
+    <definedName name="paymentItem7">'出力イメージ '!$H$2:$H$8</definedName>
+    <definedName name="paymentItem7_info1">'出力イメージ '!$H$3</definedName>
+    <definedName name="paymentItem7_info2">'出力イメージ '!$H$4</definedName>
+    <definedName name="paymentItem7_info3">'出力イメージ '!$H$5</definedName>
+    <definedName name="paymentItem7_info4">'出力イメージ '!$H$6</definedName>
+    <definedName name="paymentItem7_info5">'出力イメージ '!$H$7</definedName>
+    <definedName name="paymentItem7_info6">'出力イメージ '!$H$8</definedName>
+    <definedName name="paymentItem7_name">'出力イメージ '!$H$2</definedName>
+    <definedName name="paymentItem8">'出力イメージ '!$I$2:$I$8</definedName>
+    <definedName name="paymentItem8_info1">'出力イメージ '!$I$3</definedName>
+    <definedName name="paymentItem8_info2">'出力イメージ '!$I$4</definedName>
+    <definedName name="paymentItem8_info3">'出力イメージ '!$I$5</definedName>
+    <definedName name="paymentItem8_info4">'出力イメージ '!$I$6</definedName>
+    <definedName name="paymentItem8_info5">'出力イメージ '!$I$7</definedName>
+    <definedName name="paymentItem8_info6">'出力イメージ '!$I$8</definedName>
+    <definedName name="paymentItem8_name">'出力イメージ '!$I$2</definedName>
+    <definedName name="paymentItem9">'出力イメージ '!$J$2:$J$8</definedName>
+    <definedName name="paymentItem9_info1">'出力イメージ '!$J$3</definedName>
+    <definedName name="paymentItem9_info2">'出力イメージ '!$J$4</definedName>
+    <definedName name="paymentItem9_info3">'出力イメージ '!$J$5</definedName>
+    <definedName name="paymentItem9_info4">'出力イメージ '!$J$6</definedName>
+    <definedName name="paymentItem9_info5">'出力イメージ '!$J$7</definedName>
+    <definedName name="paymentItem9_info6">'出力イメージ '!$J$8</definedName>
+    <definedName name="paymentItem9_name">'出力イメージ '!$J$2</definedName>
     <definedName name="paymentRow">'出力イメージ '!$A$2:$J$8</definedName>
     <definedName name="PG単価" localSheetId="0">[8]明細合計!#REF!</definedName>
     <definedName name="PG単価">[8]明細合計!#REF!</definedName>
@@ -124,6 +295,15 @@
     <definedName name="processingDate">'出力イメージ '!$D$1</definedName>
     <definedName name="QuitDaicho" localSheetId="0">[9]!QuitDaicho</definedName>
     <definedName name="QuitDaicho">[9]!QuitDaicho</definedName>
+    <definedName name="reportItem1_name">'出力イメージ '!$B$21</definedName>
+    <definedName name="reportItem2_name">'出力イメージ '!$C$21</definedName>
+    <definedName name="reportItem3_name">'出力イメージ '!$D$21</definedName>
+    <definedName name="reportItem4_name">'出力イメージ '!$E$21</definedName>
+    <definedName name="reportItem5_name">'出力イメージ '!$F$21</definedName>
+    <definedName name="reportItem6_name">'出力イメージ '!$G$21</definedName>
+    <definedName name="reportItem7_name">'出力イメージ '!$H$21</definedName>
+    <definedName name="reportItem8_name">'出力イメージ '!$I$21</definedName>
+    <definedName name="reportItem9_name">'出力イメージ '!$J$21</definedName>
     <definedName name="reportRow">'出力イメージ '!$A$21:$J$21</definedName>
     <definedName name="SE単価" localSheetId="0">[8]明細合計!#REF!</definedName>
     <definedName name="SE単価">[8]明細合計!#REF!</definedName>
@@ -132,6 +312,7 @@
     <definedName name="SS単価" localSheetId="0">#REF!</definedName>
     <definedName name="SS単価">#REF!</definedName>
     <definedName name="statement">'出力イメージ '!$A$1</definedName>
+    <definedName name="statement_layout">'出力イメージ '!$A$1:$J$21</definedName>
     <definedName name="STEP概算" localSheetId="0">#REF!</definedName>
     <definedName name="STEP概算">#REF!</definedName>
     <definedName name="ＳＷ" localSheetId="0">#REF!</definedName>
@@ -306,624 +487,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="58">
-  <si>
-    <t>【明細書コード　明細書名称】</t>
-    <rPh sb="8" eb="11">
-      <t>メイサイショ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>基準年月：9999年99月</t>
-    <rPh sb="0" eb="4">
-      <t>キジュンネンゲツ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ツキ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目1</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目2</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目3</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目4</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目5</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目6</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目7</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給項目8</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウモク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>課税合計</t>
-    <rPh sb="0" eb="2">
-      <t>カゼイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ゴウケイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>合計対象内</t>
-    <rPh sb="0" eb="2">
-      <t>ゴウケイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ナイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>合計対象外</t>
-    <rPh sb="0" eb="2">
-      <t>ゴウケイ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>タイショウガイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>手入力</t>
-    <rPh sb="0" eb="1">
-      <t>テ</t>
-    </rPh>
-    <rPh sb="1" eb="3">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>個人情報参照</t>
-    <rPh sb="0" eb="2">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>サンショウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>計算式</t>
-    <rPh sb="0" eb="3">
-      <t>ケイサンシキ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>賃金テーブル</t>
-    <rPh sb="0" eb="2">
-      <t>チンギン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>共通金額</t>
-    <rPh sb="0" eb="2">
-      <t>キョウツウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キンガク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>手入力　　　交通機関</t>
-    <rPh sb="0" eb="1">
-      <t>テ</t>
-    </rPh>
-    <rPh sb="1" eb="3">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>コウツウ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>キカン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>個人情報参照　通勤費</t>
-    <rPh sb="0" eb="2">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ツウキン</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ヒ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>計算式　　　交通用具</t>
-    <rPh sb="0" eb="3">
-      <t>ケイサンシキ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>コウツウ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヨウグ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>参照：支給個人金額01</t>
-    <rPh sb="0" eb="2">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>キンガク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>式：計算式01</t>
-    <rPh sb="0" eb="1">
-      <t>シキ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>ケイサンシキ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>表：賃金テーブル01</t>
-    <rPh sb="0" eb="1">
-      <t>ヒョウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>チンギン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>金額：20,000円</t>
-    <rPh sb="0" eb="2">
-      <t>キンガク</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>エン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>参照：支給個人金額02</t>
-    <rPh sb="0" eb="2">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>シキュウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>キンガク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>式：計算式02</t>
-    <rPh sb="0" eb="1">
-      <t>シキ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>ケイサンシキ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>按分設定：なし</t>
-    <rPh sb="0" eb="2">
-      <t>アンブン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>按分設定：按分する</t>
-    <rPh sb="0" eb="2">
-      <t>アンブン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>アンブン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>按分設定：月一回支給</t>
-    <rPh sb="0" eb="2">
-      <t>アンブン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ツキ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>イッカイ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>シキュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>エラー設定：なし</t>
-    <rPh sb="3" eb="5">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>エラー設定：あり</t>
-    <rPh sb="3" eb="5">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>アラーム設定：なし</t>
-    <rPh sb="4" eb="6">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>アラーム設定：あり</t>
-    <rPh sb="4" eb="6">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>健康保険</t>
-    <rPh sb="0" eb="2">
-      <t>ケンコウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ホケン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>厚生年金</t>
-    <rPh sb="0" eb="2">
-      <t>コウセイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ネンキン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>厚生年金基金</t>
-    <rPh sb="0" eb="2">
-      <t>コウセイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ネンキン</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>キキン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>雇用保険</t>
-    <rPh sb="0" eb="2">
-      <t>コヨウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ホケン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>社会保険合計</t>
-    <rPh sb="0" eb="2">
-      <t>シャカイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ホケン</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ゴウケイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>課税対象額</t>
-    <rPh sb="0" eb="2">
-      <t>カゼイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ガク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>所得税</t>
-    <rPh sb="0" eb="3">
-      <t>ショトクゼイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>住民税</t>
-    <rPh sb="0" eb="3">
-      <t>ジュウミンゼイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>要勤務日数</t>
-    <rPh sb="0" eb="1">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="1" eb="3">
-      <t>キンム</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ニッスウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>出勤日数</t>
-    <rPh sb="0" eb="2">
-      <t>シュッキン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ニッスウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>出勤時間</t>
-    <rPh sb="0" eb="2">
-      <t>シュッキン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジカン</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>欠勤日数</t>
-    <rPh sb="0" eb="2">
-      <t>ケッキン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ニッスウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>年休使用数</t>
-    <rPh sb="0" eb="2">
-      <t>ネンキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>スウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>年休残数</t>
-    <rPh sb="0" eb="2">
-      <t>ネンキュウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ザンスウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>遅刻回数</t>
-    <rPh sb="0" eb="2">
-      <t>チコク</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>カイスウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>早退回数</t>
-    <rPh sb="0" eb="2">
-      <t>ソウタイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>カイスウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>課税対象累計</t>
-    <rPh sb="0" eb="2">
-      <t>カゼイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>タイショウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ルイケイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>端数預金額</t>
-    <rPh sb="0" eb="2">
-      <t>ハスウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ヨキン</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ガク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給1</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給2</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給3</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給4</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>支給5</t>
-    <rPh sb="0" eb="2">
-      <t>シキュウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>差引支給額</t>
-    <rPh sb="0" eb="5">
-      <t>サシヒキシキュウガク</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,12 +517,6 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -45208,13 +44768,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" s="2"/>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D1" s="3"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -45224,201 +44779,87 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="6"/>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="6"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="6"/>
-      <c r="B6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="6"/>
-      <c r="B7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="10"/>
-      <c r="B8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="2"/>
@@ -45433,30 +44874,14 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
@@ -45509,171 +44934,75 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="6"/>
-      <c r="B15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="10"/>
-      <c r="B16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
-      <c r="B20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" ht="27" customHeight="1">
       <c r="A21" s="11"/>
-      <c r="B21" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="B21" s="12"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>

<commit_message>
qmm019p: update export excel
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/明細レイアウトの作成.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/明細レイアウトの作成.xlsx
@@ -47,6 +47,7 @@
     <definedName name="AAAA" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="abc" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="ADD_COPY句">#N/A</definedName>
+    <definedName name="attendHead">'出力イメージ '!$A$18:$A$20</definedName>
     <definedName name="attendItem1">'出力イメージ '!$B$18:$B$20</definedName>
     <definedName name="attendItem1_info1">'出力イメージ '!$B$19</definedName>
     <definedName name="attendItem1_info2">'出力イメージ '!$B$20</definedName>
@@ -83,6 +84,7 @@
     <definedName name="attendItem9_info1">'出力イメージ '!$J$19</definedName>
     <definedName name="attendItem9_info2">'出力イメージ '!$J$20</definedName>
     <definedName name="attendItem9_name">'出力イメージ '!$J$18</definedName>
+    <definedName name="attendLabel">'出力イメージ '!$A$19</definedName>
     <definedName name="attendRow">'出力イメージ '!$A$18:$J$20</definedName>
     <definedName name="b" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
     <definedName name="ｂｂｂ" hidden="1">{"VIEW1",#N/A,FALSE,"懸案事項";"VIEW2",#N/A,FALSE,"懸案事項"}</definedName>
@@ -102,6 +104,7 @@
     <definedName name="C保守単価" localSheetId="0">#REF!</definedName>
     <definedName name="C保守単価">#REF!</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
+    <definedName name="deductionHead">'出力イメージ '!$A$10:$A$16</definedName>
     <definedName name="deductionItem1">'出力イメージ '!$B$10:$B$16</definedName>
     <definedName name="deductionItem1_info1">'出力イメージ '!$B$11</definedName>
     <definedName name="deductionItem1_info2">'出力イメージ '!$B$12</definedName>
@@ -174,6 +177,7 @@
     <definedName name="deductionItem9_info5">'出力イメージ '!$J$15</definedName>
     <definedName name="deductionItem9_info6">'出力イメージ '!$J$16</definedName>
     <definedName name="deductionItem9_name">'出力イメージ '!$J$10</definedName>
+    <definedName name="deductionLabel">'出力イメージ '!$A$12</definedName>
     <definedName name="deductionRow">'出力イメージ '!$A$10:$J$16</definedName>
     <definedName name="def" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="e" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
@@ -217,6 +221,7 @@
     <definedName name="OPT_YES">[4]!OPT_YES</definedName>
     <definedName name="Ｏホ" localSheetId="0">#REF!</definedName>
     <definedName name="Ｏホ">#REF!</definedName>
+    <definedName name="paymentHead">'出力イメージ '!$A$2:$A$8</definedName>
     <definedName name="paymentItem1">'出力イメージ '!$B$2:$B$8</definedName>
     <definedName name="paymentItem1_info1">'出力イメージ '!$B$3</definedName>
     <definedName name="paymentItem1_info2">'出力イメージ '!$B$4</definedName>
@@ -289,6 +294,7 @@
     <definedName name="paymentItem9_info5">'出力イメージ '!$J$7</definedName>
     <definedName name="paymentItem9_info6">'出力イメージ '!$J$8</definedName>
     <definedName name="paymentItem9_name">'出力イメージ '!$J$2</definedName>
+    <definedName name="paymentLabel">'出力イメージ '!$A$4</definedName>
     <definedName name="paymentRow">'出力イメージ '!$A$2:$J$8</definedName>
     <definedName name="PG単価" localSheetId="0">#REF!</definedName>
     <definedName name="PG単価">#REF!</definedName>
@@ -299,6 +305,7 @@
     <definedName name="processingDate">'出力イメージ '!$D$1</definedName>
     <definedName name="QuitDaicho" localSheetId="0">[5]!QuitDaicho</definedName>
     <definedName name="QuitDaicho">[5]!QuitDaicho</definedName>
+    <definedName name="reportHead">'出力イメージ '!$A$21</definedName>
     <definedName name="reportItem1_name">'出力イメージ '!$B$21</definedName>
     <definedName name="reportItem2_name">'出力イメージ '!$C$21</definedName>
     <definedName name="reportItem3_name">'出力イメージ '!$D$21</definedName>
@@ -491,6 +498,10 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
@@ -499,7 +510,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +544,13 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="MS Mincho"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -621,7 +639,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -653,11 +671,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="justify" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -680,259 +707,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>6569</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9525" y="257175"/>
-          <a:ext cx="285750" cy="733425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" vert="wordArtVertRtl" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="800">
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-            </a:rPr>
-            <a:t>支　　　給</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>124811</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>118242</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9525" y="1238250"/>
-          <a:ext cx="285750" cy="733425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" vert="wordArtVertRtl" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="800">
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-            </a:rPr>
-            <a:t>控　　　除</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>124811</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9525" y="2228850"/>
-          <a:ext cx="285750" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" vert="wordArtVertRtl" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="800">
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-            </a:rPr>
-            <a:t>勤怠</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>8283</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>16566</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1657</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="テキスト ボックス 4"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9525" y="2495550"/>
-          <a:ext cx="285750" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" vert="wordArtVertRtl" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="800">
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-            </a:rPr>
-            <a:t>記事</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44743,7 +44517,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="6"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -44755,7 +44529,7 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="6"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -44767,7 +44541,7 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="6"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -44779,7 +44553,7 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="6"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -44838,7 +44612,7 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="6"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -44850,7 +44624,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="6"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -44862,7 +44636,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="6"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -44874,7 +44648,7 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="6"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -44910,7 +44684,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="6"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -44922,7 +44696,7 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="6"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -44935,17 +44709,22 @@
     </row>
     <row r="21" spans="1:10" ht="26.25" customHeight="1">
       <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A19:A20"/>
+  </mergeCells>
   <phoneticPr fontId="4"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>
@@ -44955,6 +44734,5 @@
 &amp;C&amp;"ＭＳ 明朝,Regular"&amp;14明細書レイアウト&amp;R&amp;"ＭＳ 明朝,Regular"&amp;D　&amp;T
 &amp;N</oddHeader>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QMM019P: #130322: Edit header hiện thị page index
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/明細レイアウトの作成.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/明細レイアウトの作成.xlsx
@@ -498,10 +498,6 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
@@ -674,6 +670,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="justify" indent="1"/>
     </xf>
@@ -682,9 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -44473,7 +44469,9 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="9.75"/>
   <cols>
@@ -44517,7 +44515,7 @@
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -44529,7 +44527,7 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -44541,7 +44539,7 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -44553,7 +44551,7 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -44612,7 +44610,7 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="12"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -44624,7 +44622,7 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -44636,7 +44634,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -44648,7 +44646,7 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -44684,7 +44682,7 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -44696,7 +44694,7 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="14"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -44709,15 +44707,15 @@
     </row>
     <row r="21" spans="1:10" ht="26.25" customHeight="1">
       <c r="A21" s="11"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -44732,7 +44730,7 @@
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ 明朝,Regular"&amp;8ログイン会社名称&amp;"Meiryo UI,Regular"&amp;10
 &amp;C&amp;"ＭＳ 明朝,Regular"&amp;14明細書レイアウト&amp;R&amp;"ＭＳ 明朝,Regular"&amp;D　&amp;T
-&amp;N</oddHeader>
+&amp;P</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>